<commit_message>
Commit canges fom sanjeev
</commit_message>
<xml_diff>
--- a/APTAutomationProject_demoBranch/src/com/saksoft/qa/datalibrary/APT_MCN_CreateAccessCoreDevice_TestData.xlsx
+++ b/APTAutomationProject_demoBranch/src/com/saksoft/qa/datalibrary/APT_MCN_CreateAccessCoreDevice_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9000" windowHeight="915" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9000" windowHeight="915" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="WDMCPE" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="257">
   <si>
     <t>Name</t>
   </si>
@@ -751,28 +751,7 @@
     <t>Dev_SW_02</t>
   </si>
   <si>
-    <t>accessRouteest033</t>
-  </si>
-  <si>
-    <t>12.25.4.03</t>
-  </si>
-  <si>
-    <t>Rt76</t>
-  </si>
-  <si>
-    <t>ARST</t>
-  </si>
-  <si>
-    <t>Uh8</t>
-  </si>
-  <si>
-    <t>UJHUY67</t>
-  </si>
-  <si>
     <t>KA45</t>
-  </si>
-  <si>
-    <t>devceEdited984</t>
   </si>
   <si>
     <t>Jay35</t>
@@ -802,6 +781,33 @@
     <t>Need to update in edit device pafge for:
 new premise
 new Site</t>
+  </si>
+  <si>
+    <t>accessRouteest034</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>12.25.4.04</t>
+  </si>
+  <si>
+    <t>IN_UI1</t>
+  </si>
+  <si>
+    <t>U87</t>
+  </si>
+  <si>
+    <t>AR_PE</t>
+  </si>
+  <si>
+    <t>Rt77</t>
+  </si>
+  <si>
+    <t>de_Edit_84</t>
+  </si>
+  <si>
+    <t>edit67</t>
   </si>
 </sst>
 </file>
@@ -2832,13 +2838,13 @@
         <v>22</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>159</v>
@@ -3177,13 +3183,13 @@
         <v>22</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>159</v>
@@ -3597,7 +3603,7 @@
         <v>24</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="AA2" s="5" t="s">
         <v>15</v>
@@ -3742,8 +3748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS2"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AY1" sqref="AY1"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BR2" sqref="BR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4019,7 +4025,7 @@
     </row>
     <row r="2" spans="1:71" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>28</v>
@@ -4028,7 +4034,7 @@
         <v>142</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>249</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>143</v>
@@ -4070,7 +4076,7 @@
         <v>140</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>6</v>
@@ -4094,10 +4100,10 @@
         <v>143</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="AB2" s="5" t="s">
         <v>15</v>
@@ -4106,25 +4112,25 @@
         <v>22</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AE2" s="5" t="s">
         <v>143</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="AI2" s="8" t="s">
         <v>74</v>
       </c>
       <c r="AJ2" s="8" t="s">
-        <v>114</v>
+        <v>256</v>
       </c>
       <c r="AK2" s="8" t="s">
         <v>6</v>
@@ -4242,7 +4248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4253,7 +4259,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -5875,7 +5881,7 @@
         <v>22</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="AI2" s="5" t="s">
         <v>24</v>

</xml_diff>